<commit_message>
trying to merge again
</commit_message>
<xml_diff>
--- a/DailyStandupMeeting.xlsx
+++ b/DailyStandupMeeting.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://w2shared-my.sharepoint.com/personal/dave_sushames01_student_wandw_ac_nz/Documents/Documents/Testing and Secure Coding/GroupAssignment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="357" documentId="8_{85551688-011D-426A-89B3-D88759670DA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4DE8854B-2EB9-4A12-9219-9A8E6C9DA35A}"/>
+  <xr:revisionPtr revIDLastSave="365" documentId="8_{85551688-011D-426A-89B3-D88759670DA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{609FA781-279B-48F4-9EF7-DAAEB1161C76}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{989269EE-47AD-4604-BA2D-335F5F79A16A}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="66">
   <si>
     <t>Question</t>
   </si>
@@ -230,6 +230,12 @@
   </si>
   <si>
     <t>Team disheartened to learn that Whitebox wasn't required, after spending so much effort on them. Re-learning how Unit tests work.</t>
+  </si>
+  <si>
+    <t>Static Code Analysis</t>
+  </si>
+  <si>
+    <t>More auto tests</t>
   </si>
 </sst>
 </file>
@@ -29786,7 +29792,7 @@
   <dimension ref="B2:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30038,7 +30044,7 @@
   <dimension ref="B2:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30088,7 +30094,9 @@
         <v>10</v>
       </c>
       <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
+      <c r="E4" s="11" t="s">
+        <v>64</v>
+      </c>
       <c r="F4" s="11"/>
       <c r="G4" s="17"/>
       <c r="H4" s="17"/>
@@ -30099,7 +30107,9 @@
         <v>11</v>
       </c>
       <c r="D5" s="11"/>
-      <c r="E5" s="8"/>
+      <c r="E5" s="8" t="s">
+        <v>54</v>
+      </c>
       <c r="F5" s="18"/>
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
@@ -30110,7 +30120,9 @@
         <v>12</v>
       </c>
       <c r="D6" s="11"/>
-      <c r="E6" s="15"/>
+      <c r="E6" s="8" t="s">
+        <v>54</v>
+      </c>
       <c r="F6" s="15"/>
       <c r="G6" s="15"/>
       <c r="H6" s="15"/>
@@ -30123,7 +30135,9 @@
         <v>10</v>
       </c>
       <c r="D7" s="11"/>
-      <c r="E7" s="17"/>
+      <c r="E7" s="17" t="s">
+        <v>65</v>
+      </c>
       <c r="F7" s="17"/>
       <c r="G7" s="17"/>
       <c r="H7" s="17"/>
@@ -30134,7 +30148,9 @@
         <v>11</v>
       </c>
       <c r="D8" s="18"/>
-      <c r="E8" s="8"/>
+      <c r="E8" s="17" t="s">
+        <v>65</v>
+      </c>
       <c r="F8" s="17"/>
       <c r="G8" s="8"/>
       <c r="H8" s="8"/>
@@ -30145,7 +30161,9 @@
         <v>12</v>
       </c>
       <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
+      <c r="E9" s="17" t="s">
+        <v>65</v>
+      </c>
       <c r="F9" s="15"/>
       <c r="G9" s="15"/>
       <c r="H9" s="15"/>
@@ -30162,7 +30180,9 @@
       </c>
       <c r="E10" s="17"/>
       <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
+      <c r="G10" s="17" t="s">
+        <v>55</v>
+      </c>
       <c r="H10" s="17"/>
     </row>
     <row r="11" spans="2:8" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -30175,7 +30195,9 @@
         <v>7</v>
       </c>
       <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
+      <c r="G11" s="17" t="s">
+        <v>55</v>
+      </c>
       <c r="H11" s="8"/>
     </row>
     <row r="12" spans="2:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
all documentation done. Yes, ALL of it.
</commit_message>
<xml_diff>
--- a/DailyStandupMeeting.xlsx
+++ b/DailyStandupMeeting.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://w2shared-my.sharepoint.com/personal/dave_sushames01_student_wandw_ac_nz/Documents/Documents/Testing and Secure Coding/GroupAssignment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="365" documentId="8_{85551688-011D-426A-89B3-D88759670DA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{609FA781-279B-48F4-9EF7-DAAEB1161C76}"/>
+  <xr:revisionPtr revIDLastSave="389" documentId="8_{85551688-011D-426A-89B3-D88759670DA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BB130FC0-8E4B-4709-BA9A-1293FBD57CEB}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{989269EE-47AD-4604-BA2D-335F5F79A16A}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="76">
   <si>
     <t>Question</t>
   </si>
@@ -199,9 +199,6 @@
     <t>Static code analysis</t>
   </si>
   <si>
-    <t>Getting stuck into the tests</t>
-  </si>
-  <si>
     <t>Auto tests</t>
   </si>
   <si>
@@ -232,10 +229,43 @@
     <t>Team disheartened to learn that Whitebox wasn't required, after spending so much effort on them. Re-learning how Unit tests work.</t>
   </si>
   <si>
-    <t>Static Code Analysis</t>
+    <t>More auto tests</t>
   </si>
   <si>
-    <t>More auto tests</t>
+    <t>Finished Static Code Analysis</t>
+  </si>
+  <si>
+    <t>Finished Auto tests</t>
+  </si>
+  <si>
+    <t>Presentation slides</t>
+  </si>
+  <si>
+    <t>Last minute documentation</t>
+  </si>
+  <si>
+    <t>Getting stuck into the testing</t>
+  </si>
+  <si>
+    <t>Finishing off testing and getting onto documentation</t>
+  </si>
+  <si>
+    <t>Last minute frenzy to get the assignment done on time.</t>
+  </si>
+  <si>
+    <t>Documentation done</t>
+  </si>
+  <si>
+    <t>Finished presentation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finishing off Test Report Conclusion </t>
+  </si>
+  <si>
+    <t>Finished test report</t>
+  </si>
+  <si>
+    <t>Had some issues with github</t>
   </si>
 </sst>
 </file>
@@ -1511,7 +1541,7 @@
     <row r="14" spans="1:26" ht="42.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="1"/>
       <c r="B14" s="19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C14" s="20"/>
       <c r="D14" s="20"/>
@@ -1593,7 +1623,7 @@
     <row r="17" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A17" s="1"/>
       <c r="B17" s="19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C17" s="20"/>
       <c r="D17" s="20"/>
@@ -1623,7 +1653,7 @@
     <row r="18" spans="1:26" ht="33" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="1"/>
       <c r="B18" s="22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C18" s="23"/>
       <c r="D18" s="23"/>
@@ -29252,8 +29282,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E390CA3-3D5C-4385-B851-BBF959B643D1}">
   <dimension ref="B2:H18"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29468,7 +29498,7 @@
     </row>
     <row r="15" spans="2:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="22" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C15" s="23"/>
       <c r="D15" s="23"/>
@@ -29488,7 +29518,7 @@
     </row>
     <row r="17" spans="2:8" ht="27.75" x14ac:dyDescent="0.35">
       <c r="B17" s="19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C17" s="20"/>
       <c r="D17" s="20"/>
@@ -29499,7 +29529,7 @@
     </row>
     <row r="18" spans="2:8" ht="27.75" x14ac:dyDescent="0.25">
       <c r="B18" s="22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C18" s="23"/>
       <c r="D18" s="23"/>
@@ -29529,8 +29559,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A670754B-33A0-4207-85BD-63F0E6FB13ED}">
   <dimension ref="B2:H18"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B18" sqref="B17:E18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29756,7 +29786,7 @@
     </row>
     <row r="17" spans="2:5" ht="27.75" x14ac:dyDescent="0.35">
       <c r="B17" s="19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C17" s="20"/>
       <c r="D17" s="20"/>
@@ -29764,7 +29794,7 @@
     </row>
     <row r="18" spans="2:5" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B18" s="22" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C18" s="23"/>
       <c r="D18" s="23"/>
@@ -29791,8 +29821,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F577788E-DDBE-4FB8-9001-CCFE30A56FC6}">
   <dimension ref="B2:H18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29914,7 +29944,7 @@
       <c r="F8" s="17"/>
       <c r="G8" s="8"/>
       <c r="H8" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="2:8" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -29929,7 +29959,7 @@
       <c r="F9" s="15"/>
       <c r="G9" s="15"/>
       <c r="H9" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="2:8" ht="27" x14ac:dyDescent="0.25">
@@ -29997,7 +30027,7 @@
     </row>
     <row r="15" spans="2:8" ht="27.75" x14ac:dyDescent="0.25">
       <c r="B15" s="22" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="C15" s="23"/>
       <c r="D15" s="23"/>
@@ -30008,7 +30038,7 @@
     </row>
     <row r="17" spans="2:5" ht="27.75" x14ac:dyDescent="0.35">
       <c r="B17" s="19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C17" s="20"/>
       <c r="D17" s="20"/>
@@ -30016,7 +30046,7 @@
     </row>
     <row r="18" spans="2:5" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="37" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C18" s="38"/>
       <c r="D18" s="38"/>
@@ -30043,8 +30073,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0D50EA9-52A9-43FA-A599-959B6893304B}">
   <dimension ref="B2:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30060,7 +30090,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="29" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E2" s="30"/>
       <c r="F2" s="30"/>
@@ -30097,9 +30127,15 @@
       <c r="E4" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="F4" s="11"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
+      <c r="F4" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="G4" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="5" spans="2:8" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="33"/>
@@ -30108,11 +30144,17 @@
       </c>
       <c r="D5" s="11"/>
       <c r="E5" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
-      <c r="F5" s="18"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
+      <c r="F5" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="G5" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="6" spans="2:8" ht="55.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="34"/>
@@ -30121,11 +30163,17 @@
       </c>
       <c r="D6" s="11"/>
       <c r="E6" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
+      <c r="F6" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="G6" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="7" spans="2:8" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="35" t="s">
@@ -30136,23 +30184,31 @@
       </c>
       <c r="D7" s="11"/>
       <c r="E7" s="17" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
+      <c r="F7" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="G7" s="17" t="s">
+        <v>67</v>
+      </c>
       <c r="H7" s="17"/>
     </row>
-    <row r="8" spans="2:8" ht="27" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:8" ht="36" x14ac:dyDescent="0.25">
       <c r="B8" s="36"/>
       <c r="C8" s="6" t="s">
         <v>11</v>
       </c>
       <c r="D8" s="18"/>
       <c r="E8" s="17" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
-      <c r="F8" s="17"/>
-      <c r="G8" s="8"/>
+      <c r="F8" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>66</v>
+      </c>
       <c r="H8" s="8"/>
     </row>
     <row r="9" spans="2:8" ht="60.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -30162,10 +30218,14 @@
       </c>
       <c r="D9" s="15"/>
       <c r="E9" s="17" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
+      <c r="F9" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="G9" s="15" t="s">
+        <v>73</v>
+      </c>
       <c r="H9" s="15"/>
     </row>
     <row r="10" spans="2:8" ht="54" x14ac:dyDescent="0.25">
@@ -30176,13 +30236,13 @@
         <v>10</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17" t="s">
-        <v>55</v>
+      <c r="F10" s="17" t="s">
+        <v>54</v>
       </c>
+      <c r="G10" s="17"/>
       <c r="H10" s="17"/>
     </row>
     <row r="11" spans="2:8" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -30194,9 +30254,11 @@
       <c r="E11" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="F11" s="8"/>
-      <c r="G11" s="17" t="s">
-        <v>55</v>
+      <c r="F11" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>75</v>
       </c>
       <c r="H11" s="8"/>
     </row>
@@ -30236,7 +30298,9 @@
       <c r="H14" s="1"/>
     </row>
     <row r="15" spans="2:8" ht="27.75" x14ac:dyDescent="0.25">
-      <c r="B15" s="22"/>
+      <c r="B15" s="22" t="s">
+        <v>69</v>
+      </c>
       <c r="C15" s="23"/>
       <c r="D15" s="23"/>
       <c r="E15" s="24"/>
@@ -30246,14 +30310,16 @@
     </row>
     <row r="17" spans="2:5" ht="27.75" x14ac:dyDescent="0.35">
       <c r="B17" s="19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C17" s="20"/>
       <c r="D17" s="20"/>
       <c r="E17" s="21"/>
     </row>
     <row r="18" spans="2:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B18" s="22"/>
+      <c r="B18" s="22" t="s">
+        <v>70</v>
+      </c>
       <c r="C18" s="23"/>
       <c r="D18" s="23"/>
       <c r="E18" s="24"/>

</xml_diff>